<commit_message>
added cumulative diagram of total batfly counts v infected
</commit_message>
<xml_diff>
--- a/3T/Data/EDA/cumulative_number_found_on_a_yearly_basis.xlsx
+++ b/3T/Data/EDA/cumulative_number_found_on_a_yearly_basis.xlsx
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreypan/Documents/teamlaboul/3T/Data/EDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DDAB6CE9-27BB-F040-A20D-7671FD90DCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1A515F07-DA96-404A-AB40-C61BC2718198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="cumulative_number_ofund_on_a_ye" sheetId="1" r:id="rId1"/>
+    <sheet name="Cumulative counts comparison" sheetId="3" r:id="rId1"/>
+    <sheet name="cumulative infected samples" sheetId="2" r:id="rId2"/>
+    <sheet name="cumulative total recorded sampl" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cumulative_number_ofund_on_a_ye!$A$1:$C$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'cumulative infected samples'!$A$1:$C$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'cumulative total recorded sampl'!$A$1:$C$18</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Cumulative counts comparison'!$A$2:$A$23</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Cumulative counts comparison'!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Cumulative counts comparison'!$B$2:$B$23</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Cumulative counts comparison'!$C$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Cumulative counts comparison'!$C$2:$C$23</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Cumulative counts comparison'!$A$2:$A$23</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Cumulative counts comparison'!$B$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Cumulative counts comparison'!$B$2:$B$23</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Cumulative counts comparison'!$C$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Cumulative counts comparison'!$C$2:$C$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Year</t>
   </si>
@@ -45,6 +58,18 @@
   </si>
   <si>
     <t>Cumulative count</t>
+  </si>
+  <si>
+    <t>Cumulative count of recorded (infected + uninfected)</t>
+  </si>
+  <si>
+    <t>Cumulative count of infected batflies</t>
+  </si>
+  <si>
+    <t>Infection count</t>
+  </si>
+  <si>
+    <t>Record count</t>
   </si>
 </sst>
 </file>
@@ -609,6 +634,777 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cumulative counts comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative counts comparison'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative count of infected batflies</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative counts comparison'!$A$2:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative counts comparison'!$B$2:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>519</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>592</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5286-CD4E-A70A-735C3DD41B09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cumulative counts comparison'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumulative count of recorded (infected + uninfected)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cumulative counts comparison'!$A$2:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cumulative counts comparison'!$C$2:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>665</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>869</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1028</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1907</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5265</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5675</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5679</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5828</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5861</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5946</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10585</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12035</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14953</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15300</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15937</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16043</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16545</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5286-CD4E-A70A-735C3DD41B09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="351797903"/>
+        <c:axId val="352094495"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="351797903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="352094495"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="352094495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351797903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
                 <a:gradFill>
                   <a:gsLst>
@@ -690,7 +1486,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>cumulative_number_ofund_on_a_ye!$A$1</c:f>
+              <c:f>'cumulative infected samples'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -780,7 +1576,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>cumulative_number_ofund_on_a_ye!$A$2:$A$18</c:f>
+              <c:f>'cumulative infected samples'!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -840,7 +1636,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>cumulative_number_ofund_on_a_ye!$C$2:$C$18</c:f>
+              <c:f>'cumulative infected samples'!$C$2:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -894,6 +1690,597 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>592</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A593-8843-A4BB-181A9668112A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2079829408"/>
+        <c:axId val="365684271"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2079829408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="365684271"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="365684271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2079829408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                <a:gradFill>
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="85000"/>
+                        <a:lumOff val="15000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="0"/>
+                </a:gradFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Recorded Batflies Over Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'cumulative total recorded sampl'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'cumulative total recorded sampl'!$A$2:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'cumulative total recorded sampl'!$C$2:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>665</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>869</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1028</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1907</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5265</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5675</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5679</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5828</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5861</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5946</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10585</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12035</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14953</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15300</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15937</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16043</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1150,6 +2537,83 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1190,6 +2654,531 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="280">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="234">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1699,7 +3688,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="234">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9575">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" cap="all" spc="0" baseline="0">
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91F47CBF-3685-4BE6-3E20-9B35345CF415}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1711,6 +4251,49 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1736964-2B1D-1546-A522-0435D8EC0ABB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
@@ -2037,10 +4620,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1993</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1994</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>665</v>
+      </c>
+      <c r="D3">
+        <v>656</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1995</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>869</v>
+      </c>
+      <c r="D4">
+        <v>204</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1996</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>910</v>
+      </c>
+      <c r="D5">
+        <v>41</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1998</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1028</v>
+      </c>
+      <c r="D6">
+        <v>118</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1999</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>1768</v>
+      </c>
+      <c r="D7">
+        <v>740</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2000</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1907</v>
+      </c>
+      <c r="D8">
+        <v>139</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2004</v>
+      </c>
+      <c r="B9">
+        <v>101</v>
+      </c>
+      <c r="C9">
+        <v>5265</v>
+      </c>
+      <c r="D9">
+        <v>3358</v>
+      </c>
+      <c r="E9">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2006</v>
+      </c>
+      <c r="B10">
+        <v>107</v>
+      </c>
+      <c r="C10">
+        <v>5675</v>
+      </c>
+      <c r="D10">
+        <v>410</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2007</v>
+      </c>
+      <c r="B11">
+        <v>107</v>
+      </c>
+      <c r="C11">
+        <v>5679</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2008</v>
+      </c>
+      <c r="B12">
+        <v>107</v>
+      </c>
+      <c r="C12">
+        <v>5696</v>
+      </c>
+      <c r="D12">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2009</v>
+      </c>
+      <c r="B13">
+        <v>122</v>
+      </c>
+      <c r="C13">
+        <v>5828</v>
+      </c>
+      <c r="D13">
+        <v>132</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2010</v>
+      </c>
+      <c r="B14">
+        <v>133</v>
+      </c>
+      <c r="C14">
+        <v>5861</v>
+      </c>
+      <c r="D14">
+        <v>33</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2011</v>
+      </c>
+      <c r="B15">
+        <v>144</v>
+      </c>
+      <c r="C15">
+        <v>5946</v>
+      </c>
+      <c r="D15">
+        <v>85</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2012</v>
+      </c>
+      <c r="B16">
+        <v>229</v>
+      </c>
+      <c r="C16">
+        <v>9999</v>
+      </c>
+      <c r="D16">
+        <v>4053</v>
+      </c>
+      <c r="E16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2013</v>
+      </c>
+      <c r="B17">
+        <v>270</v>
+      </c>
+      <c r="C17">
+        <v>10585</v>
+      </c>
+      <c r="D17">
+        <v>586</v>
+      </c>
+      <c r="E17">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2014</v>
+      </c>
+      <c r="B18">
+        <v>339</v>
+      </c>
+      <c r="C18">
+        <v>12035</v>
+      </c>
+      <c r="D18">
+        <v>1450</v>
+      </c>
+      <c r="E18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2015</v>
+      </c>
+      <c r="B19">
+        <v>460</v>
+      </c>
+      <c r="C19">
+        <v>14953</v>
+      </c>
+      <c r="D19">
+        <v>2918</v>
+      </c>
+      <c r="E19">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2016</v>
+      </c>
+      <c r="B20">
+        <v>519</v>
+      </c>
+      <c r="C20">
+        <v>15300</v>
+      </c>
+      <c r="D20">
+        <v>347</v>
+      </c>
+      <c r="E20">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2017</v>
+      </c>
+      <c r="B21">
+        <v>556</v>
+      </c>
+      <c r="C21">
+        <v>15937</v>
+      </c>
+      <c r="D21">
+        <v>637</v>
+      </c>
+      <c r="E21">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2018</v>
+      </c>
+      <c r="B22">
+        <v>576</v>
+      </c>
+      <c r="C22">
+        <v>16043</v>
+      </c>
+      <c r="D22">
+        <v>106</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2019</v>
+      </c>
+      <c r="B23">
+        <v>592</v>
+      </c>
+      <c r="C23">
+        <v>16545</v>
+      </c>
+      <c r="D23">
+        <v>502</v>
+      </c>
+      <c r="E23">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" activeCellId="1" sqref="A1:A1048576 B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2252,4 +5248,278 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1993</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1994</v>
+      </c>
+      <c r="B3">
+        <v>656</v>
+      </c>
+      <c r="C3">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1995</v>
+      </c>
+      <c r="B4">
+        <v>204</v>
+      </c>
+      <c r="C4">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1996</v>
+      </c>
+      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1998</v>
+      </c>
+      <c r="B6">
+        <v>118</v>
+      </c>
+      <c r="C6">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1999</v>
+      </c>
+      <c r="B7">
+        <v>740</v>
+      </c>
+      <c r="C7">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2000</v>
+      </c>
+      <c r="B8">
+        <v>139</v>
+      </c>
+      <c r="C8">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2004</v>
+      </c>
+      <c r="B9">
+        <v>3358</v>
+      </c>
+      <c r="C9">
+        <v>5265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2006</v>
+      </c>
+      <c r="B10">
+        <v>410</v>
+      </c>
+      <c r="C10">
+        <v>5675</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2007</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>5679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2008</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>5696</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2009</v>
+      </c>
+      <c r="B13">
+        <v>132</v>
+      </c>
+      <c r="C13">
+        <v>5828</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2010</v>
+      </c>
+      <c r="B14">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>5861</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2011</v>
+      </c>
+      <c r="B15">
+        <v>85</v>
+      </c>
+      <c r="C15">
+        <v>5946</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2012</v>
+      </c>
+      <c r="B16">
+        <v>4053</v>
+      </c>
+      <c r="C16">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2013</v>
+      </c>
+      <c r="B17">
+        <v>586</v>
+      </c>
+      <c r="C17">
+        <v>10585</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2014</v>
+      </c>
+      <c r="B18">
+        <v>1450</v>
+      </c>
+      <c r="C18">
+        <v>12035</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2015</v>
+      </c>
+      <c r="B19">
+        <v>2918</v>
+      </c>
+      <c r="C19">
+        <v>14953</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2016</v>
+      </c>
+      <c r="B20">
+        <v>347</v>
+      </c>
+      <c r="C20">
+        <v>15300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2017</v>
+      </c>
+      <c r="B21">
+        <v>637</v>
+      </c>
+      <c r="C21">
+        <v>15937</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2018</v>
+      </c>
+      <c r="B22">
+        <v>106</v>
+      </c>
+      <c r="C22">
+        <v>16043</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2019</v>
+      </c>
+      <c r="B23">
+        <v>502</v>
+      </c>
+      <c r="C23">
+        <v>16545</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C18">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C23">
+      <sortCondition ref="A1:A23"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added biopy test output and the line graph (area)
</commit_message>
<xml_diff>
--- a/3T/Data/EDA/cumulative_number_found_on_a_yearly_basis.xlsx
+++ b/3T/Data/EDA/cumulative_number_found_on_a_yearly_basis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreypan/Documents/teamlaboul/3T/Data/EDA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey\Documents\GitHub\teamlaboul\3T\Data\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2E721651-B5C4-5748-A8A8-21AAFF5F4F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6B56DF-8CA4-413F-841A-6A59ABD90C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cumulative counts comparison" sheetId="3" r:id="rId1"/>
@@ -20,16 +20,6 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'cumulative infected samples'!$A$1:$C$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'cumulative total recorded sampl'!$A$1:$C$18</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'Cumulative counts comparison'!$A$2:$A$23</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Cumulative counts comparison'!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Cumulative counts comparison'!$B$2:$B$23</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Cumulative counts comparison'!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Cumulative counts comparison'!$C$2:$C$23</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Cumulative counts comparison'!$A$2:$A$23</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Cumulative counts comparison'!$B$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Cumulative counts comparison'!$B$2:$B$23</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Cumulative counts comparison'!$C$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Cumulative counts comparison'!$C$2:$C$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -75,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -648,8 +638,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Cumulative counts comparison</a:t>
+              <a:t>Cumulative Counts of</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Bat Flies (infected vs total)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -740,6 +735,447 @@
             <a:effectLst/>
           </c:spPr>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.6275730014360938E-2"/>
+                  <c:y val="-1.6682113067655237E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.2242817423540315E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5104110191572596E-17"/>
+                  <c:y val="-2.0389249304911955E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.2242817423540315E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.5739588319766712E-4"/>
+                  <c:y val="-2.7803521779425393E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-1.6682113067655237E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.0208220383145192E-17"/>
+                  <c:y val="-2.7803521779425393E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.5739588319770225E-4"/>
+                  <c:y val="-3.3364226135310607E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.5739588319770225E-4"/>
+                  <c:y val="-2.7803521779425529E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.5739588319770225E-4"/>
+                  <c:y val="-2.5949953660797033E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.7803521779425529E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-3.3364226135310607E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8721876495930365E-3"/>
+                  <c:y val="-2.7803521779425393E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.7803521779425393E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.5739588319756184E-4"/>
+                  <c:y val="-2.9657089898053754E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.5949953660797033E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-4.2632066728452406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.5739588319770225E-4"/>
+                  <c:y val="-4.2632066728452274E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4041644076629038E-16"/>
+                  <c:y val="-3.1510658016682111E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4041644076629038E-16"/>
+                  <c:y val="-4.4485634847080631E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.573958831977163E-3"/>
+                  <c:y val="-4.4485634847080763E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -966,32 +1402,12 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent6">
@@ -1003,6 +1419,468 @@
             <a:effectLst/>
           </c:spPr>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.8779380367099502E-3"/>
+                  <c:y val="-2.4245866894743409E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000029-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.7587195944439149E-17"/>
+                  <c:y val="-3.5436267000009396E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000028-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-3.7301333684220422E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002A-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-4.4761600421064501E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000027-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9186253578066335E-3"/>
+                  <c:y val="-4.6626667105275528E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000026-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.8779380367099853E-3"/>
+                  <c:y val="-6.900746731580791E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000024-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.796563394516549E-3"/>
+                  <c:y val="-7.2737600684229825E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000025-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.5931267890331674E-4"/>
+                  <c:y val="-0.14734026805267081"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.9186253578066335E-3"/>
+                  <c:y val="-0.16226080152635883"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000017-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9186253578066335E-3"/>
+                  <c:y val="-0.16599093489478087"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000018-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-0.16412586821056985"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000019-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.7965633945165134E-3"/>
+                  <c:y val="-0.15666560147372582"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.7965633945165837E-3"/>
+                  <c:y val="-0.15853066815793679"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001A-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.6745014312266041E-3"/>
+                  <c:y val="-0.16785600157899203"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001B-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.5931267890317611E-4"/>
+                  <c:y val="-0.25551413573690995"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001C-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.7151887523232172E-3"/>
+                  <c:y val="-0.27229973589480916"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001D-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.7151887523233577E-3"/>
+                  <c:y val="-0.29841066947376338"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001E-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.7151887523232172E-3"/>
+                  <c:y val="-0.37674347021062626"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001F-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.8372507156132669E-3"/>
+                  <c:y val="-0.39725920373694745"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000023-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.7965633945165837E-3"/>
+                  <c:y val="-0.40098933710536949"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000022-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.5931267890331674E-4"/>
+                  <c:y val="-0.41217973721063561"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000021-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3430377504646575E-2"/>
+                  <c:y val="-0.4177749372632687"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000020-5528-4B3A-9849-D11DB028DA81}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1041,20 +1919,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -1232,6 +2097,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1297,6 +2217,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4209,7 +5188,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
+      <xdr:colOff>628650</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
@@ -4324,9 +5303,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4364,7 +5343,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4470,7 +5449,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4612,29 +5591,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.875" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4651,7 +5630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1993</v>
       </c>
@@ -4668,7 +5647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1994</v>
       </c>
@@ -4685,7 +5664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1995</v>
       </c>
@@ -4702,7 +5681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1996</v>
       </c>
@@ -4719,7 +5698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1998</v>
       </c>
@@ -4736,7 +5715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1999</v>
       </c>
@@ -4753,7 +5732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2000</v>
       </c>
@@ -4770,7 +5749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2004</v>
       </c>
@@ -4787,7 +5766,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2006</v>
       </c>
@@ -4804,7 +5783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2007</v>
       </c>
@@ -4821,7 +5800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2008</v>
       </c>
@@ -4838,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2009</v>
       </c>
@@ -4855,7 +5834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2010</v>
       </c>
@@ -4872,7 +5851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -4889,7 +5868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>
@@ -4906,7 +5885,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2013</v>
       </c>
@@ -4923,7 +5902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2014</v>
       </c>
@@ -4940,7 +5919,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2015</v>
       </c>
@@ -4957,7 +5936,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2016</v>
       </c>
@@ -4974,7 +5953,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2017</v>
       </c>
@@ -4991,7 +5970,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2018</v>
       </c>
@@ -5008,7 +5987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -5032,16 +6011,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" activeCellId="1" sqref="A1:A1048576 B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5052,7 +6031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1994</v>
       </c>
@@ -5063,7 +6042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1995</v>
       </c>
@@ -5074,7 +6053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1998</v>
       </c>
@@ -5085,7 +6064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2000</v>
       </c>
@@ -5096,7 +6075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -5107,7 +6086,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2006</v>
       </c>
@@ -5118,7 +6097,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2009</v>
       </c>
@@ -5129,7 +6108,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2010</v>
       </c>
@@ -5140,7 +6119,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -5151,7 +6130,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2012</v>
       </c>
@@ -5162,7 +6141,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2013</v>
       </c>
@@ -5173,7 +6152,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2014</v>
       </c>
@@ -5184,7 +6163,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2015</v>
       </c>
@@ -5195,7 +6174,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2016</v>
       </c>
@@ -5206,7 +6185,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2017</v>
       </c>
@@ -5217,7 +6196,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2018</v>
       </c>
@@ -5228,7 +6207,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -5240,7 +6219,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C18">
+  <autoFilter ref="A1:C18" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
       <sortCondition ref="A1:A18"/>
     </sortState>
@@ -5251,16 +6230,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5271,7 +6250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1993</v>
       </c>
@@ -5282,7 +6261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1994</v>
       </c>
@@ -5293,7 +6272,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1995</v>
       </c>
@@ -5304,7 +6283,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1996</v>
       </c>
@@ -5315,7 +6294,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1998</v>
       </c>
@@ -5326,7 +6305,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1999</v>
       </c>
@@ -5337,7 +6316,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2000</v>
       </c>
@@ -5348,7 +6327,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2004</v>
       </c>
@@ -5359,7 +6338,7 @@
         <v>5265</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2006</v>
       </c>
@@ -5370,7 +6349,7 @@
         <v>5675</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2007</v>
       </c>
@@ -5381,7 +6360,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2008</v>
       </c>
@@ -5392,7 +6371,7 @@
         <v>5696</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2009</v>
       </c>
@@ -5403,7 +6382,7 @@
         <v>5828</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2010</v>
       </c>
@@ -5414,7 +6393,7 @@
         <v>5861</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -5425,7 +6404,7 @@
         <v>5946</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>
@@ -5436,7 +6415,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2013</v>
       </c>
@@ -5447,7 +6426,7 @@
         <v>10585</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2014</v>
       </c>
@@ -5458,7 +6437,7 @@
         <v>12035</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2015</v>
       </c>
@@ -5469,7 +6448,7 @@
         <v>14953</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2016</v>
       </c>
@@ -5480,7 +6459,7 @@
         <v>15300</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2017</v>
       </c>
@@ -5491,7 +6470,7 @@
         <v>15937</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2018</v>
       </c>
@@ -5502,7 +6481,7 @@
         <v>16043</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -5514,7 +6493,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C18">
+  <autoFilter ref="A1:C18" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C23">
       <sortCondition ref="A1:A23"/>
     </sortState>

</xml_diff>